<commit_message>
Added Data Table:  Reference Details , Data Table:  Examination Result to DATABASE
</commit_message>
<xml_diff>
--- a/Acceptance Tests/Dispatcher.xlsx
+++ b/Acceptance Tests/Dispatcher.xlsx
@@ -1,29 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26905"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asaf/Desktop/GHealth-System/Acceptance Tests/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="DataBase" sheetId="2" r:id="rId1"/>
     <sheet name="Dispatcher" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="266">
   <si>
     <t xml:space="preserve">Use Case: </t>
   </si>
@@ -836,6 +828,66 @@
   </si>
   <si>
     <t>Data Table: Medical field</t>
+  </si>
+  <si>
+    <t>Data Table:  Reference Details</t>
+  </si>
+  <si>
+    <t>Examination Code</t>
+  </si>
+  <si>
+    <t>Urgency</t>
+  </si>
+  <si>
+    <t>1.7.16</t>
+  </si>
+  <si>
+    <t>2.7.16</t>
+  </si>
+  <si>
+    <t>3.7.16</t>
+  </si>
+  <si>
+    <t>Data Table:  Examination Result</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Picture</t>
+  </si>
+  <si>
+    <t>attached</t>
+  </si>
+  <si>
+    <t>not attached</t>
+  </si>
+  <si>
+    <t>catheterization, positive</t>
+  </si>
+  <si>
+    <t>Scoliosis , There is severe Scoliosis.</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>first priority</t>
+  </si>
+  <si>
+    <t>Upper Respiratory Tract Infection , he has it</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>He bearly breath</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -846,7 +898,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -854,7 +906,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -863,7 +915,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -871,7 +923,7 @@
       <b/>
       <u/>
       <sz val="14"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -879,20 +931,20 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1166,7 +1218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1356,6 +1408,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1445,7 +1506,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1480,7 +1541,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1657,7 +1718,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1665,30 +1726,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H90"/>
+  <dimension ref="A2:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="J107" sqref="J107:J108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>114</v>
       </c>
@@ -2026,12 +2087,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
         <v>7</v>
       </c>
@@ -2101,12 +2162,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
         <v>131</v>
       </c>
@@ -2166,12 +2227,12 @@
       <c r="B31" s="39"/>
       <c r="C31" s="40"/>
     </row>
-    <row r="32" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="46" t="s">
         <v>244</v>
       </c>
@@ -2239,12 +2300,12 @@
       <c r="B42" s="39"/>
       <c r="C42" s="43"/>
     </row>
-    <row r="43" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="44" t="s">
         <v>92</v>
       </c>
@@ -2294,12 +2355,12 @@
       <c r="B49" s="39"/>
       <c r="C49" s="40"/>
     </row>
-    <row r="51" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="29" t="s">
         <v>7</v>
       </c>
@@ -2409,12 +2470,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="29" t="s">
         <v>76</v>
       </c>
@@ -2652,12 +2713,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="29" t="s">
         <v>111</v>
       </c>
@@ -2671,7 +2732,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="17">
         <v>302632195</v>
       </c>
@@ -2685,7 +2746,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="17">
         <v>302632195</v>
       </c>
@@ -2699,7 +2760,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>305003659</v>
       </c>
@@ -2713,7 +2774,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>305003659</v>
       </c>
@@ -2727,7 +2788,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>305003659</v>
       </c>
@@ -2741,7 +2802,7 @@
         <v>0.39583333333333331</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>312143969</v>
       </c>
@@ -2755,7 +2816,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>312143969</v>
       </c>
@@ -2767,6 +2828,148 @@
       </c>
       <c r="D90" s="58">
         <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="67" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="B94" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="C94" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="D94" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="E94" s="69" t="s">
+        <v>248</v>
+      </c>
+      <c r="F94" s="69" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="15">
+        <v>302632195</v>
+      </c>
+      <c r="B95" s="15">
+        <v>1004</v>
+      </c>
+      <c r="C95" s="15">
+        <v>90000</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="E95" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="F95" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="15">
+        <v>305003659</v>
+      </c>
+      <c r="B96" s="15">
+        <v>1002</v>
+      </c>
+      <c r="C96" s="15">
+        <v>90001</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="E96" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="F96" s="70" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="15">
+        <v>200940997</v>
+      </c>
+      <c r="B97" s="15">
+        <v>1001</v>
+      </c>
+      <c r="C97" s="15">
+        <v>90002</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="E97" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="F97" s="70" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="71"/>
+      <c r="B98" s="71"/>
+      <c r="C98" s="71"/>
+      <c r="D98" s="71"/>
+      <c r="E98" s="71"/>
+      <c r="F98" s="71"/>
+    </row>
+    <row r="100" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="67" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="B101" s="69" t="s">
+        <v>253</v>
+      </c>
+      <c r="C101" s="69" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="15">
+        <v>90000</v>
+      </c>
+      <c r="B102" s="70" t="s">
+        <v>257</v>
+      </c>
+      <c r="C102" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="15">
+        <v>90001</v>
+      </c>
+      <c r="B103" s="70" t="s">
+        <v>258</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="15">
+        <v>90002</v>
+      </c>
+      <c r="B104" s="70" t="s">
+        <v>262</v>
+      </c>
+      <c r="C104" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -2789,7 +2992,7 @@
     <hyperlink ref="G15" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId17"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -2801,21 +3004,21 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.375" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="66"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
@@ -2823,7 +3026,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
@@ -2831,13 +3034,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="24"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>3</v>
       </c>
@@ -2845,7 +3048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>13</v>
       </c>
@@ -2853,7 +3056,7 @@
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
     </row>
-    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>14</v>
       </c>
@@ -2867,7 +3070,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="100.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -2881,7 +3084,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="100.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
@@ -2895,7 +3098,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
@@ -2909,7 +3112,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -2923,7 +3126,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>46</v>
       </c>
@@ -2937,14 +3140,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="65" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="66"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
         <v>0</v>
       </c>
@@ -2952,7 +3155,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
         <v>1</v>
       </c>
@@ -2960,13 +3163,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="24"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
         <v>3</v>
       </c>
@@ -2974,7 +3177,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>13</v>
       </c>
@@ -2982,7 +3185,7 @@
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
     </row>
-    <row r="24" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>14</v>
       </c>
@@ -2996,7 +3199,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>49</v>
       </c>
@@ -3010,7 +3213,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
@@ -3024,7 +3227,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>51</v>
       </c>
@@ -3038,7 +3241,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>52</v>
       </c>
@@ -3052,7 +3255,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="86.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>53</v>
       </c>
@@ -3066,7 +3269,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>23</v>
       </c>
@@ -3080,14 +3283,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="65" t="s">
         <v>72</v>
       </c>
       <c r="B33" s="66"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="27" t="s">
         <v>0</v>
       </c>
@@ -3095,7 +3298,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="28" t="s">
         <v>1</v>
       </c>
@@ -3103,13 +3306,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B36" s="24"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="28" t="s">
         <v>3</v>
       </c>
@@ -3117,7 +3320,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="22" t="s">
         <v>13</v>
       </c>
@@ -3125,7 +3328,7 @@
       <c r="C39" s="40"/>
       <c r="D39" s="41"/>
     </row>
-    <row r="40" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
         <v>14</v>
       </c>
@@ -3139,7 +3342,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="91" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="86.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>185</v>
       </c>
@@ -3153,7 +3356,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>186</v>
       </c>
@@ -3167,7 +3370,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="86.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>188</v>
       </c>
@@ -3181,7 +3384,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>23</v>
       </c>
@@ -3195,14 +3398,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="65" t="s">
         <v>196</v>
       </c>
       <c r="B47" s="66"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="27" t="s">
         <v>0</v>
       </c>
@@ -3210,7 +3413,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="28" t="s">
         <v>1</v>
       </c>
@@ -3218,13 +3421,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B50" s="24"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="28" t="s">
         <v>3</v>
       </c>
@@ -3232,12 +3435,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
         <v>14</v>
       </c>
@@ -3251,7 +3454,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="86.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>198</v>
       </c>
@@ -3265,7 +3468,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="106" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="114.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>199</v>
       </c>
@@ -3279,7 +3482,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>206</v>
       </c>
@@ -3293,7 +3496,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>23</v>
       </c>
@@ -3307,14 +3510,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="65" t="s">
         <v>202</v>
       </c>
       <c r="B61" s="66"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="s">
         <v>0</v>
       </c>
@@ -3322,7 +3525,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="28" t="s">
         <v>1</v>
       </c>
@@ -3330,13 +3533,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B64" s="24"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="28" t="s">
         <v>3</v>
       </c>
@@ -3344,12 +3547,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="32" t="s">
         <v>14</v>
       </c>
@@ -3363,7 +3566,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>216</v>
       </c>
@@ -3377,7 +3580,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="166" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="186" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>218</v>
       </c>
@@ -3391,7 +3594,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="59" t="s">
         <v>220</v>
       </c>
@@ -3405,7 +3608,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>23</v>
       </c>
@@ -3419,14 +3622,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="65" t="s">
         <v>204</v>
       </c>
       <c r="B75" s="66"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="27" t="s">
         <v>0</v>
       </c>
@@ -3434,7 +3637,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="28" t="s">
         <v>1</v>
       </c>
@@ -3442,13 +3645,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B78" s="24"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="28" t="s">
         <v>3</v>
       </c>
@@ -3456,12 +3659,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="32" t="s">
         <v>14</v>
       </c>
@@ -3475,7 +3678,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="86.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>223</v>
       </c>
@@ -3489,7 +3692,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="106" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="114.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>235</v>
       </c>
@@ -3503,7 +3706,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="86.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>230</v>
       </c>
@@ -3517,7 +3720,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Lab Manager Testing Update
</commit_message>
<xml_diff>
--- a/Acceptance Tests/Dispatcher.xlsx
+++ b/Acceptance Tests/Dispatcher.xlsx
@@ -1402,12 +1402,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1417,6 +1411,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1718,7 +1718,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1728,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="J107" sqref="J107:J108"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2831,27 +2831,27 @@
       </c>
     </row>
     <row r="93" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="67" t="s">
+      <c r="A93" s="65" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="68" t="s">
+      <c r="A94" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="B94" s="68" t="s">
+      <c r="B94" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="C94" s="69" t="s">
+      <c r="C94" s="67" t="s">
         <v>247</v>
       </c>
-      <c r="D94" s="69" t="s">
+      <c r="D94" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="E94" s="69" t="s">
+      <c r="E94" s="67" t="s">
         <v>248</v>
       </c>
-      <c r="F94" s="69" t="s">
+      <c r="F94" s="67" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2891,7 +2891,7 @@
       <c r="E96" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="F96" s="70" t="s">
+      <c r="F96" s="68" t="s">
         <v>265</v>
       </c>
     </row>
@@ -2911,31 +2911,31 @@
       <c r="E97" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="F97" s="70" t="s">
+      <c r="F97" s="68" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="71"/>
-      <c r="B98" s="71"/>
-      <c r="C98" s="71"/>
-      <c r="D98" s="71"/>
-      <c r="E98" s="71"/>
-      <c r="F98" s="71"/>
+      <c r="A98" s="69"/>
+      <c r="B98" s="69"/>
+      <c r="C98" s="69"/>
+      <c r="D98" s="69"/>
+      <c r="E98" s="69"/>
+      <c r="F98" s="69"/>
     </row>
     <row r="100" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="67" t="s">
+      <c r="A100" s="65" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="69" t="s">
+      <c r="A101" s="67" t="s">
         <v>247</v>
       </c>
-      <c r="B101" s="69" t="s">
+      <c r="B101" s="67" t="s">
         <v>253</v>
       </c>
-      <c r="C101" s="69" t="s">
+      <c r="C101" s="67" t="s">
         <v>254</v>
       </c>
     </row>
@@ -2943,7 +2943,7 @@
       <c r="A102" s="15">
         <v>90000</v>
       </c>
-      <c r="B102" s="70" t="s">
+      <c r="B102" s="68" t="s">
         <v>257</v>
       </c>
       <c r="C102" s="15" t="s">
@@ -2954,7 +2954,7 @@
       <c r="A103" s="15">
         <v>90001</v>
       </c>
-      <c r="B103" s="70" t="s">
+      <c r="B103" s="68" t="s">
         <v>258</v>
       </c>
       <c r="C103" s="15" t="s">
@@ -2965,7 +2965,7 @@
       <c r="A104" s="15">
         <v>90002</v>
       </c>
-      <c r="B104" s="70" t="s">
+      <c r="B104" s="68" t="s">
         <v>262</v>
       </c>
       <c r="C104" s="15" t="s">
@@ -3000,8 +3000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3013,10 +3013,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="71"/>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
@@ -3142,10 +3142,10 @@
     </row>
     <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="65" t="s">
+      <c r="A17" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="66"/>
+      <c r="B17" s="71"/>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
@@ -3285,10 +3285,10 @@
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="65" t="s">
+      <c r="A33" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="66"/>
+      <c r="B33" s="71"/>
     </row>
     <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="27" t="s">
@@ -3400,10 +3400,10 @@
     </row>
     <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="65" t="s">
+      <c r="A47" s="70" t="s">
         <v>196</v>
       </c>
-      <c r="B47" s="66"/>
+      <c r="B47" s="71"/>
     </row>
     <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="27" t="s">
@@ -3512,10 +3512,10 @@
     </row>
     <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="65" t="s">
+      <c r="A61" s="70" t="s">
         <v>202</v>
       </c>
-      <c r="B61" s="66"/>
+      <c r="B61" s="71"/>
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="s">
@@ -3624,10 +3624,10 @@
     </row>
     <row r="74" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="65" t="s">
+      <c r="A75" s="70" t="s">
         <v>204</v>
       </c>
-      <c r="B75" s="66"/>
+      <c r="B75" s="71"/>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="27" t="s">

</xml_diff>